<commit_message>
Removal of unused methods.
</commit_message>
<xml_diff>
--- a/input_scenario_grid.xlsx
+++ b/input_scenario_grid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\GitHub\timessim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scava\Documents\GitHub\timessim\timessim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16E7524-3EBF-474C-9F70-D143D00593D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3A1E8D-0AA3-4F64-958D-0DC84CE5065B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CBD37C51-DE11-477E-A99E-920B88BDC9F9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CBD37C51-DE11-477E-A99E-920B88BDC9F9}"/>
   </bookViews>
   <sheets>
     <sheet name="grid_layout" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>BS</t>
   </si>
@@ -156,15 +156,6 @@
   </si>
   <si>
     <t>UE 23</t>
-  </si>
-  <si>
-    <t>Machine 9</t>
-  </si>
-  <si>
-    <t>Machine 11</t>
-  </si>
-  <si>
-    <t>Machine 10</t>
   </si>
 </sst>
 </file>
@@ -549,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3898D35-7679-4280-9259-21E890B7A44A}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,64 +742,57 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
-        <v>22</v>
-      </c>
-      <c r="C12" s="1">
         <v>14.5</v>
       </c>
+      <c r="C12" s="3">
+        <v>5.5</v>
+      </c>
       <c r="D12" s="1">
         <v>1</v>
-      </c>
-      <c r="E12" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1">
-        <v>22</v>
+        <v>5.5</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E13" s="1">
-        <v>2</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1">
-        <v>5.5</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="1">
-        <v>2</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1">
-        <v>14.5</v>
-      </c>
-      <c r="C15" s="3">
-        <v>5.5</v>
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>10</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -816,43 +800,41 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>5.5</v>
+        <v>14.5</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1">
-        <v>19</v>
+        <v>5.5</v>
       </c>
       <c r="C17" s="1">
-        <v>10</v>
+        <v>14.5</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
+        <v>5.5</v>
       </c>
       <c r="C18" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -860,13 +842,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1">
-        <v>14.5</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -874,13 +856,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>5.5</v>
       </c>
       <c r="C20" s="1">
-        <v>14.5</v>
+        <v>5.5</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -888,13 +870,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
-        <v>5.5</v>
+        <v>14.5</v>
       </c>
       <c r="C21" s="1">
-        <v>1</v>
+        <v>14.5</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -902,13 +884,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1">
         <v>10</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -916,13 +898,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1">
-        <v>5.5</v>
+        <v>14.5</v>
       </c>
       <c r="C23" s="1">
-        <v>5.5</v>
+        <v>19</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -930,13 +912,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1">
-        <v>14.5</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1">
-        <v>14.5</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -944,13 +926,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C25" s="1">
-        <v>19</v>
+        <v>5.5</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -958,27 +940,28 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1">
-        <v>14.5</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1">
-        <v>19</v>
+        <v>5.5</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C27" s="1">
-        <v>1</v>
+        <v>14.5</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
@@ -986,13 +969,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B28" s="1">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C28" s="1">
-        <v>5.5</v>
+        <v>14.5</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
@@ -1000,28 +983,27 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1">
-        <v>5.5</v>
+        <v>19</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
       </c>
-      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C30" s="1">
-        <v>14.5</v>
+        <v>19</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -1029,13 +1011,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B31" s="1">
-        <v>19</v>
+        <v>5.5</v>
       </c>
       <c r="C31" s="1">
-        <v>14.5</v>
+        <v>10</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -1043,10 +1025,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1">
-        <v>19</v>
+        <v>5.5</v>
       </c>
       <c r="C32" s="1">
         <v>19</v>
@@ -1057,13 +1039,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1">
-        <v>1</v>
+        <v>14.5</v>
       </c>
       <c r="C33" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
@@ -1071,10 +1053,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B34" s="1">
-        <v>5.5</v>
+        <v>14.5</v>
       </c>
       <c r="C34" s="1">
         <v>10</v>
@@ -1082,61 +1064,19 @@
       <c r="D34" s="1">
         <v>1</v>
       </c>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1">
-        <v>5.5</v>
+        <v>19</v>
       </c>
       <c r="C35" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="1">
-        <v>14.5</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="1">
-        <v>14.5</v>
-      </c>
-      <c r="C37" s="1">
-        <v>10</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1</v>
-      </c>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="1">
-        <v>19</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1</v>
-      </c>
-      <c r="D38" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>